<commit_message>
Fix blank page generation by filtering sectPr elements
Fixed critical issue where 3 Excel rows generated 5 Word pages with blank pages.
Root cause was copying sectPr (section properties) elements from templates which
create section breaks. Added logic to skip sectPr elements during template copying,
maintaining document structure while preventing blank page generation.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Format for ARN change.xlsx
+++ b/Format for ARN change.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabit\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ARN CHANGE FORM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C1F7F53-29D4-4657-81E8-07445DDDBBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FA484C-7BB0-4747-830B-8E9CF9BC5C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{21AEF9C9-B1C3-4310-98CC-BF395E1997F3}"/>
+    <workbookView xWindow="-100" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{21AEF9C9-B1C3-4310-98CC-BF395E1997F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Mutual Fund</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t xml:space="preserve">ASHAR </t>
+  </si>
+  <si>
+    <t>Nippon Large Cap Fund</t>
+  </si>
+  <si>
+    <t>CMRPM0258F</t>
+  </si>
+  <si>
+    <t>Nippon Small Cap Fund</t>
+  </si>
+  <si>
+    <t>AGHPM9964E</t>
+  </si>
+  <si>
+    <t>AMAN</t>
   </si>
 </sst>
 </file>
@@ -445,21 +460,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505F1F9E-DC77-4E41-B145-A9537599CBE6}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -485,6 +500,34 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>11110000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>